<commit_message>
[JPADSandbox_v2] Testing AVL external job class
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -202,42 +202,81 @@
     <t>Ixz</t>
   </si>
   <si>
-    <t>Xcg LRF</t>
+    <t>Xcg calibration factor</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Zcg calibration factor</t>
+  </si>
+  <si>
+    <t>Xcg MAC (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg MAC (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg LRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg LRF (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg BRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg BRF (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Ycg LRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg MAC (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg MAC (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg LRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg LRF (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg BRF (NOT CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Zcg BRF (CALIBRATED)</t>
+  </si>
+  <si>
+    <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
+  </si>
+  <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
+    <t>Ycg LRF (semi-wing)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (semi-wing)</t>
+  </si>
+  <si>
+    <t>Ycg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
     <t>Ycg LRF</t>
   </si>
   <si>
-    <t>Zcg LRF</t>
-  </si>
-  <si>
-    <t>Xcg BRF</t>
-  </si>
-  <si>
     <t>Ycg BRF</t>
   </si>
   <si>
-    <t>Zcg BRF</t>
-  </si>
-  <si>
-    <t>Xcg ESTIMATION METHOD COMPARISON</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>Ycg LRF (semi-wing)</t>
-  </si>
-  <si>
-    <t>Ycg BRF (semi-wing)</t>
-  </si>
-  <si>
-    <t>Ycg ESTIMATION METHOD COMPARISON</t>
-  </si>
-  <si>
     <t>Ycg LRF (semi-tail)</t>
   </si>
   <si>
@@ -247,7 +286,7 @@
     <t>TORENBEEK_1976</t>
   </si>
   <si>
-    <t>Zcg ESTIMATION METHOD COMPARISON</t>
+    <t>Zcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
 </sst>
 </file>
@@ -343,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.639942552666746</v>
+        <v>17.537354531331758</v>
       </c>
     </row>
     <row r="4">
@@ -365,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.6523756577637356</v>
+        <v>-0.7366743395896822</v>
       </c>
     </row>
     <row r="6">
@@ -381,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>44.347793563220606</v>
+        <v>41.716158714420196</v>
       </c>
     </row>
     <row r="8">
@@ -403,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-16.735038780736815</v>
+        <v>-18.89750712659457</v>
       </c>
     </row>
     <row r="10">
@@ -429,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.641768800929256</v>
+        <v>16.598447268422312</v>
       </c>
     </row>
     <row r="14">
@@ -451,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.8865111021658749</v>
+        <v>-0.9425442266839414</v>
       </c>
     </row>
     <row r="16">
@@ -467,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>18.74218390190764</v>
+        <v>17.63088013402975</v>
       </c>
     </row>
     <row r="18">
@@ -489,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-22.74118829809647</v>
+        <v>-24.17857563874324</v>
       </c>
     </row>
     <row r="20">
@@ -515,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.641768800929256</v>
+        <v>16.598447268422312</v>
       </c>
     </row>
     <row r="24">
@@ -537,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.8865111021658749</v>
+        <v>-0.9425442266839414</v>
       </c>
     </row>
     <row r="26">
@@ -553,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>18.74218390190764</v>
+        <v>17.63088013402975</v>
       </c>
     </row>
     <row r="28">
@@ -575,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-22.74118829809647</v>
+        <v>-24.17857563874324</v>
       </c>
     </row>
     <row r="30">
@@ -601,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>16.641768800929256</v>
+        <v>16.598447268422312</v>
       </c>
     </row>
     <row r="34">
@@ -623,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.8865111021658749</v>
+        <v>-0.9425442266839414</v>
       </c>
     </row>
     <row r="36">
@@ -639,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>18.74218390190764</v>
+        <v>17.63088013402975</v>
       </c>
     </row>
     <row r="38">
@@ -661,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-22.74118829809647</v>
+        <v>-24.17857563874324</v>
       </c>
     </row>
     <row r="40">
@@ -687,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>17.120534297659937</v>
+        <v>17.134977127082394</v>
       </c>
     </row>
     <row r="44">
@@ -709,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.6451145620464458</v>
+        <v>-0.6942309309452876</v>
       </c>
     </row>
     <row r="46">
@@ -725,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>31.02369541956823</v>
+        <v>31.394189486310243</v>
       </c>
     </row>
     <row r="48">
@@ -747,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-16.54877383204755</v>
+        <v>-17.80872939370766</v>
       </c>
     </row>
     <row r="50">
@@ -773,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.980173764460766</v>
+        <v>17.02597814532112</v>
       </c>
     </row>
     <row r="54">
@@ -795,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.7928508395702571</v>
+        <v>-0.7970576970723231</v>
       </c>
     </row>
     <row r="56">
@@ -811,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>27.423102818635048</v>
+        <v>28.598097748171803</v>
       </c>
     </row>
     <row r="58">
@@ -833,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-20.338572400187985</v>
+        <v>-20.446488633119543</v>
       </c>
     </row>
     <row r="60">
@@ -854,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>12.260541979316603</v>
+        <v>11.352758242551236</v>
       </c>
     </row>
     <row r="63">
@@ -865,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>27.423102818635048</v>
+        <v>28.598097748171803</v>
       </c>
     </row>
     <row r="64">
@@ -876,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>35.250538901941106</v>
+        <v>35.24673678363601</v>
       </c>
     </row>
     <row r="65">
@@ -907,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>54267.93047148815</v>
+        <v>56879.30324254191</v>
       </c>
     </row>
     <row r="70">
@@ -918,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>3095872.3845237037</v>
+        <v>2969297.017437632</v>
       </c>
     </row>
     <row r="71">
@@ -929,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>3041604.454052216</v>
+        <v>2912417.7141950903</v>
       </c>
     </row>
     <row r="72">
@@ -972,7 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>17528.990386791542</v>
+        <v>-6560.580896219946</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1025,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1008,101 +1047,221 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>16.988911111111108</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>27.647237231521256</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>16.988911111111104</v>
+        <v>27.647237231521203</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>16.988911111111108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>16.988911111111104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.988911111111104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>16.9889111111111</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>17.143322222222217</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>17.143322222222217</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
         <v>16.8345</v>
       </c>
     </row>
@@ -1117,7 +1276,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1139,133 +1298,253 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>3.978609561291834</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C3" t="n">
-        <v>5.556533960383371</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.089699723510626</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>16.14860956129183</v>
+        <v>6.089699723510626</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>5.55653396038337</v>
+        <v>3.9785418179282894</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.2499999999999998</v>
+        <v>3.978541817928289</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.148541817928287</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>16.148541817928287</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4.3629715646212155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>3.5942475579624524</v>
+        <v>5.556533960383371</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.55653396038337</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>4.998846772296348</v>
+        <v>-32.06557177137496</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C16" t="n">
+        <v>-32.06557177137496</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.2499999999999998</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.2499999999999998</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>4.3631082000119275</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.5939754358446514</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>4.998846772296348</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="n">
         <v>6.114221148470394</v>
       </c>
     </row>
@@ -1280,7 +1559,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1302,74 +1581,194 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>4.375847808880026</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16.28157473795874</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>16.545847808880023</v>
+        <v>16.281574737958696</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>4.375847808880026</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.2499999999999998</v>
+        <v>4.3758478088800254</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.545847808880023</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>16.54584780888002</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-32.06557177137496</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-32.065571771374955</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.2499999999999998</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.2499999999999996</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1384,7 +1783,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1406,111 +1805,231 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7981052333017615</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C3" t="n">
-        <v>2.269503332277167</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>448.58339069994423</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>33.39810523330176</v>
+        <v>448.58339069994423</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.269503332277167</v>
+        <v>1.7981052333017615</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.0</v>
+        <v>1.7981052333017613</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>33.39810523330176</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>33.39810523330176</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.7981052333017615</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.269503332277167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.269503332277167</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>25.65245741709997</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>25.65245741709997</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.7981052333017615</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="n">
         <v>2.2695033322771674</v>
       </c>
     </row>
@@ -1525,7 +2044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1547,111 +2066,231 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>3.4971039999999975</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C3" t="n">
-        <v>2.333199999999999</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>476.77540976411603</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>34.49710399999999</v>
+        <v>476.7754097641159</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>3.4971039999999975</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3.8531999999999984</v>
+        <v>3.497103999999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>34.49710399999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>34.49710399999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3.4971039999999975</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.333199999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>98.84404891956959</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>98.84404891956959</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.8531999999999984</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3.8531999999999984</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3.4971039999999975</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="n">
         <v>2.3331999999999993</v>
       </c>
     </row>
@@ -1666,7 +2305,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1688,7 +2327,7 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -1696,82 +2335,202 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-84.93911815369333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>12.599999999999998</v>
+        <v>-84.93911815369333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>5.999999999999999</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.5999999999999999</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12.599999999999998</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>12.599999999999998</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.999999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-41.04393186735996</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-41.04393186735996</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
         <v>74</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -1786,7 +2545,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1808,90 +2567,210 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-59.286660736593355</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>13.599999999999998</v>
+        <v>-59.286660736593355</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>5.999999999999999</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.5999999999999999</v>
+        <v>1.9999999999999998</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>13.599999999999998</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>13.599999999999998</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.999999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-41.04393186735996</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-41.04393186735996</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -1906,7 +2785,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
   <cols>
     <col min="2" max="2" width="8.0" customWidth="true"/>
     <col min="3" max="3" width="15.0" customWidth="true"/>
@@ -1928,111 +2807,231 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
-        <v>16.89037358995828</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-2.129999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12.823659727039871</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>16.890373589958276</v>
+        <v>12.823659727039827</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>16.411049221957363</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.9799999999999986</v>
+        <v>16.41104922195736</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.41104922195736</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>16.411049221957356</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>16.89037358995828</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-76.4443231029579</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-76.44432310295788</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-2.129999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-2.1299999999999986</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-2.9799999999999986</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-2.979999999999998</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>16.411049221957363</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="n">
         <v>-2.129999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[JPADSandbox] New user sandbox2.masc - Testing AVL
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
[JPADSandbox_v2] More work on AVL classes
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Small changes in AVL classes
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Little changes on AVL classes
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300_AVL/BALANCE/Balance.xlsx
@@ -382,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.537354531331758</v>
+        <v>17.532329314974604</v>
       </c>
     </row>
     <row r="4">
@@ -404,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7366743395896822</v>
+        <v>-0.741123728435491</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>41.716158714420196</v>
+        <v>41.58724956580667</v>
       </c>
     </row>
     <row r="8">
@@ -442,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-18.89750712659457</v>
+        <v>-19.0116448844938</v>
       </c>
     </row>
     <row r="10">
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.598447268422312</v>
+        <v>16.599203470659226</v>
       </c>
     </row>
     <row r="14">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.9425442266839414</v>
+        <v>-0.9449315944283343</v>
       </c>
     </row>
     <row r="16">
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>17.63088013402975</v>
+        <v>17.650278579711</v>
       </c>
     </row>
     <row r="18">
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-24.17857563874324</v>
+        <v>-24.23981748814523</v>
       </c>
     </row>
     <row r="20">
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.598447268422312</v>
+        <v>16.599203470659226</v>
       </c>
     </row>
     <row r="24">
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.9425442266839414</v>
+        <v>-0.9449315944283343</v>
       </c>
     </row>
     <row r="26">
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>17.63088013402975</v>
+        <v>17.650278579711</v>
       </c>
     </row>
     <row r="28">
@@ -614,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-24.17857563874324</v>
+        <v>-24.23981748814523</v>
       </c>
     </row>
     <row r="30">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>16.598447268422312</v>
+        <v>16.599203470659226</v>
       </c>
     </row>
     <row r="34">
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.9425442266839414</v>
+        <v>-0.9449315944283343</v>
       </c>
     </row>
     <row r="36">
@@ -678,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>17.63088013402975</v>
+        <v>17.650278579711</v>
       </c>
     </row>
     <row r="38">
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-24.17857563874324</v>
+        <v>-24.23981748814523</v>
       </c>
     </row>
     <row r="40">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>17.134977127082394</v>
+        <v>17.132888164407937</v>
       </c>
     </row>
     <row r="44">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.6942309309452876</v>
+        <v>-0.6905131041571593</v>
       </c>
     </row>
     <row r="46">
@@ -764,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>31.394189486310243</v>
+        <v>31.34060246025785</v>
       </c>
     </row>
     <row r="48">
@@ -786,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-17.80872939370766</v>
+        <v>-17.71335800034105</v>
       </c>
     </row>
     <row r="50">
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>17.02597814532112</v>
+        <v>17.024276851488253</v>
       </c>
     </row>
     <row r="54">
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.7970576970723231</v>
+        <v>-0.7940266117833963</v>
       </c>
     </row>
     <row r="56">
@@ -850,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>28.598097748171803</v>
+        <v>28.55445538057032</v>
       </c>
     </row>
     <row r="58">
@@ -872,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-20.446488633119543</v>
+        <v>-20.36873384681775</v>
       </c>
     </row>
     <row r="60">
@@ -893,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>11.352758242551236</v>
+        <v>11.410774450069002</v>
       </c>
     </row>
     <row r="63">
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>28.598097748171803</v>
+        <v>28.55445538057032</v>
       </c>
     </row>
     <row r="64">
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>35.24673678363601</v>
+        <v>35.166164044004056</v>
       </c>
     </row>
     <row r="65">
@@ -946,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>56879.30324254191</v>
+        <v>57430.90350385681</v>
       </c>
     </row>
     <row r="70">
@@ -957,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>2969297.017437632</v>
+        <v>2984198.0030505783</v>
       </c>
     </row>
     <row r="71">
@@ -968,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>2912417.7141950903</v>
+        <v>2926767.099546721</v>
       </c>
     </row>
     <row r="72">
@@ -1011,7 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>-6560.580896219946</v>
+        <v>-6714.732829158727</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.8345</v>
+        <v>16.834499999999995</v>
       </c>
     </row>
     <row r="24">
@@ -2837,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>12.823659727039871</v>
+        <v>12.948317647221725</v>
       </c>
     </row>
     <row r="6">
@@ -2848,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>12.823659727039827</v>
+        <v>12.94831764722168</v>
       </c>
     </row>
     <row r="7">
@@ -2859,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>16.411049221957363</v>
+        <v>16.41590871429195</v>
       </c>
     </row>
     <row r="8">
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>16.41104922195736</v>
+        <v>16.41590871429195</v>
       </c>
     </row>
     <row r="9">
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>16.41104922195736</v>
+        <v>16.41590871429195</v>
       </c>
     </row>
     <row r="10">
@@ -2892,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>16.411049221957356</v>
+        <v>16.41590871429195</v>
       </c>
     </row>
     <row r="11">
@@ -3011,7 +3011,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.411049221957363</v>
+        <v>16.41590871429195</v>
       </c>
     </row>
     <row r="24">

</xml_diff>